<commit_message>
Merging Projects into Core Branches
</commit_message>
<xml_diff>
--- a/raftaar-core/assets/testcase.xlsx
+++ b/raftaar-core/assets/testcase.xlsx
@@ -10,7 +10,7 @@
     <sheet name="KeywordList" sheetId="13" r:id="rId1"/>
     <sheet name="FlagsList" sheetId="23" r:id="rId2"/>
     <sheet name="Template" sheetId="20" r:id="rId3"/>
-    <sheet name="TestCases1" sheetId="12" r:id="rId4"/>
+    <sheet name="TestSuite1" sheetId="12" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="490">
   <si>
     <t>openBrowser</t>
   </si>
@@ -1114,9 +1114,6 @@
     <t>{optional}</t>
   </si>
   <si>
-    <t>{nowait}</t>
-  </si>
-  <si>
     <t>{nolog}</t>
   </si>
   <si>
@@ -1135,9 +1132,6 @@
     <t>assertAll</t>
   </si>
   <si>
-    <t>{normalize}</t>
-  </si>
-  <si>
     <t>xpath=//button[@onclick='alertFunction()']</t>
   </si>
   <si>
@@ -1484,6 +1478,21 @@
   </si>
   <si>
     <t>xpath=//*[@class='downArrow']</t>
+  </si>
+  <si>
+    <t>This will skip the particular test step</t>
+  </si>
+  <si>
+    <t>This will not log step in report</t>
+  </si>
+  <si>
+    <t>Defect ID to be attached in test case</t>
+  </si>
+  <si>
+    <t>Test.Case.030</t>
+  </si>
+  <si>
+    <t>linkText=Home</t>
   </si>
 </sst>
 </file>
@@ -2036,7 +2045,7 @@
         <v>92</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2185,10 +2194,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2236,7 +2245,7 @@
         <v>43</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2361,10 +2370,10 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -3161,18 +3170,18 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -3250,7 +3259,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3273,38 +3282,32 @@
         <v>362</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="10" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="B5" s="10"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>430</v>
-      </c>
-      <c r="B6" s="10"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="B7" s="10"/>
+        <v>428</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3387,11 +3390,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD98"/>
+  <dimension ref="A1:XFD102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E95" sqref="E95"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3442,7 +3445,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>6</v>
@@ -3616,7 +3619,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3720,7 +3723,7 @@
         <v>8</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -3756,7 +3759,7 @@
         <v>8</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -3792,7 +3795,7 @@
         <v>8</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -3862,7 +3865,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -3881,14 +3884,14 @@
         <v>56</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>345</v>
@@ -3909,7 +3912,7 @@
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>337</v>
@@ -3923,14 +3926,14 @@
         <v>346</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>349</v>
@@ -3961,7 +3964,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -3978,7 +3981,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -4002,7 +4005,7 @@
     </row>
     <row r="33" spans="1:16384" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>355</v>
@@ -4023,7 +4026,7 @@
     </row>
     <row r="34" spans="1:16384" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>355</v>
@@ -4134,7 +4137,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -20537,7 +20540,7 @@
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>2</v>
@@ -20550,7 +20553,7 @@
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -20578,10 +20581,10 @@
         <v>344</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E46" s="9">
         <v>5</v>
@@ -20604,37 +20607,37 @@
         <v>360</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="48" spans="1:16384" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -20659,7 +20662,7 @@
         <v>358</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>336</v>
@@ -20675,13 +20678,13 @@
     </row>
     <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -20692,10 +20695,10 @@
     </row>
     <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>7</v>
@@ -20709,13 +20712,13 @@
     </row>
     <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -20723,7 +20726,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
@@ -20736,13 +20739,13 @@
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
@@ -20755,13 +20758,13 @@
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>53</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
@@ -20770,11 +20773,11 @@
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>2</v>
@@ -20787,11 +20790,11 @@
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>45</v>
@@ -20806,11 +20809,11 @@
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>2</v>
@@ -20823,11 +20826,11 @@
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>45</v>
@@ -20842,17 +20845,17 @@
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>28</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
@@ -20861,30 +20864,30 @@
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
     <row r="64" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E64" s="9">
         <v>10</v>
@@ -20898,10 +20901,10 @@
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>6</v>
@@ -20910,31 +20913,31 @@
         <v>0</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>109</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>6</v>
@@ -20943,48 +20946,48 @@
         <v>0</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>113</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>117</v>
       </c>
       <c r="G69" s="12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>6</v>
@@ -20993,17 +20996,17 @@
         <v>0</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>123</v>
@@ -21011,10 +21014,10 @@
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>6</v>
@@ -21023,17 +21026,17 @@
         <v>0</v>
       </c>
       <c r="G72" s="12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>125</v>
@@ -21041,30 +21044,30 @@
     </row>
     <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>6</v>
@@ -21073,12 +21076,12 @@
         <v>0</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E76" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>44</v>
@@ -21086,10 +21089,10 @@
     </row>
     <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>6</v>
@@ -21098,29 +21101,29 @@
         <v>0</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D78" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>28</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>6</v>
@@ -21129,23 +21132,23 @@
         <v>0</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C80" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>159</v>
       </c>
       <c r="G80" s="12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C81" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>157</v>
@@ -21153,18 +21156,18 @@
     </row>
     <row r="82" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C82" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>5</v>
@@ -21175,7 +21178,7 @@
         <v>0</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H83"/>
       <c r="I83"/>
@@ -21184,12 +21187,12 @@
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D84"/>
       <c r="E84"/>
       <c r="F84" s="6" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="G84"/>
       <c r="H84"/>
@@ -21212,17 +21215,17 @@
     </row>
     <row r="86" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D86"/>
       <c r="E86" s="6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>125</v>
@@ -21235,11 +21238,11 @@
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D87"/>
       <c r="E87" s="6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>125</v>
@@ -21252,11 +21255,11 @@
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D88"/>
       <c r="E88" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>125</v>
@@ -21269,11 +21272,11 @@
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89" s="6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D89"/>
       <c r="E89" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>125</v>
@@ -21286,11 +21289,11 @@
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D90"/>
       <c r="E90" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>125</v>
@@ -21303,11 +21306,11 @@
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D91"/>
       <c r="E91" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>125</v>
@@ -21320,11 +21323,11 @@
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D92"/>
       <c r="E92" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>125</v>
@@ -21337,11 +21340,11 @@
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93" s="6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D93"/>
       <c r="E93" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>125</v>
@@ -21352,10 +21355,10 @@
     </row>
     <row r="94" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>6</v>
@@ -21364,15 +21367,15 @@
         <v>0</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C95" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F95" s="5" t="s">
         <v>2</v>
@@ -21380,33 +21383,97 @@
     </row>
     <row r="96" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C96" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F96" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C97" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F97" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="98" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C98" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F98" s="5" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="99" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+    </row>
+    <row r="100" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="6"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G100" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+    </row>
+    <row r="101" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="6"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+    </row>
+    <row r="102" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C102" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G102" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>